<commit_message>
BB_pos Beige book 부정으로 된 것 수정
</commit_message>
<xml_diff>
--- a/Fed1/doc/금리 예측 통합 데이터 정리.xlsx
+++ b/Fed1/doc/금리 예측 통합 데이터 정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitStudy\MLP_Finance_Fed\Fed1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52946ABE-785F-47DD-B1D1-3018FC24779E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9E56A1-816D-44C7-A769-1D4736B6BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AC71F577-D77B-4174-9A13-27B93AA63A31}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="171">
   <si>
     <t>연준 기준 금리 상한</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -726,6 +726,10 @@
 파일이 .xlsx라 openpyxl 모듈 설치 필요
 실제,예측,이전 컬럼의 값에 100을 곱합
 20240731일 기준 20240801 예측치가 나와 있으나 일단 제외</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beige book 긍정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -882,6 +886,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -890,9 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1223,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE7A5CC-1392-4053-90B6-52C60D5BB7CE}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1246,36 +1250,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1763,29 +1767,29 @@
       <c r="E14" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="12" t="s">
         <v>155</v>
       </c>
       <c r="I14" s="16">
         <v>20180101</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11" t="s">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1802,16 +1806,16 @@
       <c r="D15" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
@@ -1826,23 +1830,23 @@
       <c r="D16" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>151</v>
@@ -1850,16 +1854,16 @@
       <c r="D17" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" ht="33">
       <c r="A18" s="1" t="s">
@@ -1874,16 +1878,16 @@
       <c r="D18" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
@@ -1911,11 +1915,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="J14:J18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="M14:M18"/>
@@ -1926,6 +1925,11 @@
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="J14:J18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1989,7 +1993,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="49.5">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2009,7 +2013,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
@@ -2021,7 +2025,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
@@ -2031,7 +2035,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
@@ -2041,7 +2045,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
@@ -2051,7 +2055,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2061,7 +2065,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="49.5">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
@@ -2079,7 +2083,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2091,7 +2095,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2101,7 +2105,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
@@ -2111,7 +2115,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="99">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="8" t="s">
         <v>49</v>
       </c>
@@ -2129,7 +2133,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>50</v>
       </c>
@@ -2139,7 +2143,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
@@ -2149,7 +2153,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2161,7 +2165,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
@@ -2171,7 +2175,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
@@ -2181,7 +2185,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="33">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>55</v>
       </c>

</xml_diff>